<commit_message>
SVN (com) commit #8789 by scriswellwsf       CBECC 2022/25 executables, CSE v0.925.0, ruleset source and UI updates enabling residential split heat pump and air cond simulation in CSE via new Performance Map model (based on NEEP database)
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24R Tables.xlsx
+++ b/Documentation/T24Res/T24R Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFam-VCHP3\RulesetDev\Rulesets\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34198027-35FA-484E-9EBF-053CEFDA1530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFC2387-B6EA-4D9E-A08A-12634E0E1111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="1335" windowWidth="20715" windowHeight="14895" tabRatio="750" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="855" windowWidth="26535" windowHeight="15525" tabRatio="750" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T24RClimateZoneDesignDay" sheetId="9" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6712" uniqueCount="1068">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6714" uniqueCount="1069">
   <si>
     <t>;</t>
   </si>
@@ -3315,6 +3315,9 @@
   </si>
   <si>
     <t>TABLE  HtPump3_Interp_VarSpeed_Full_HeatCapRatio_COP</t>
+  </si>
+  <si>
+    <t>04/15/25 SAC - updated 2D interpolation tables based on latest NEEP-statistics spreadsheet (from BigLadder/NK)</t>
   </si>
 </sst>
 </file>
@@ -6224,8 +6227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AG402"/>
   <sheetViews>
-    <sheetView topLeftCell="A355" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D378" sqref="D378"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10731,7 +10734,7 @@
         <v>189</v>
       </c>
       <c r="O120" s="72">
-        <f t="shared" ref="O120:U129" si="49">O90</f>
+        <f t="shared" ref="O120:U126" si="49">O90</f>
         <v>1</v>
       </c>
       <c r="P120" s="61">
@@ -35685,10 +35688,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309192F8-0F3D-4CE7-AD0F-AA8B35DF48AD}">
-  <dimension ref="A1:L195"/>
+  <dimension ref="A1:L196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G184" sqref="G184"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E195" sqref="E195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35735,7 +35738,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>799</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -35767,7 +35770,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -35775,13 +35778,16 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
+      <c r="D10" t="s">
+        <v>802</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -35789,138 +35795,138 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="145" t="s">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="145" t="s">
         <v>803</v>
       </c>
-      <c r="C12" s="145"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="147" t="s">
+      <c r="C13" s="145"/>
+      <c r="D13" s="146"/>
+      <c r="E13" s="146"/>
+      <c r="F13" s="146"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="147" t="s">
         <v>804</v>
       </c>
-      <c r="D13" s="147" t="s">
+      <c r="D14" s="147" t="s">
         <v>805</v>
       </c>
-      <c r="E13" s="147" t="s">
+      <c r="E14" s="147" t="s">
         <v>806</v>
       </c>
-      <c r="F13" s="147" t="s">
+      <c r="F14" s="147" t="s">
         <v>807</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>808</v>
-      </c>
-      <c r="D14" s="196">
-        <v>-0.32406970650566153</v>
-      </c>
-      <c r="E14" s="196">
-        <v>1.304995981404673</v>
-      </c>
-      <c r="F14" s="196">
-        <v>0.12655634584261771</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D15" s="196">
-        <v>-0.1194657608023873</v>
+        <v>-0.32406970650566153</v>
       </c>
       <c r="E15" s="196">
-        <v>0.50962874336215891</v>
+        <v>1.304995981404673</v>
       </c>
       <c r="F15" s="196">
-        <v>4.6810878271605683E-2</v>
+        <v>0.12655634584261771</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D16" s="196">
-        <v>6.5998782097587902E-2</v>
+        <v>-0.1194657608023873</v>
       </c>
       <c r="E16" s="196">
-        <v>2.8367979164842292</v>
+        <v>0.50962874336215891</v>
       </c>
       <c r="F16" s="196">
-        <v>5.4463218005817222E-2</v>
+        <v>4.6810878271605683E-2</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
+        <v>812</v>
+      </c>
+      <c r="D17" s="196">
+        <v>6.5998782097587902E-2</v>
+      </c>
+      <c r="E17" s="196">
+        <v>2.8367979164842292</v>
+      </c>
+      <c r="F17" s="196">
+        <v>5.4463218005817222E-2</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>814</v>
       </c>
-      <c r="D17" s="196">
-        <f>D15/D14</f>
+      <c r="D18" s="196">
+        <f>D16/D15</f>
         <v>0.36864217297737523</v>
       </c>
-      <c r="E17" s="196">
-        <f>E15-D15/D14*E14</f>
+      <c r="E18" s="196">
+        <f>E16-D16/D15*E15</f>
         <v>2.8552189050397914E-2</v>
       </c>
-      <c r="F17" s="196">
-        <v>0</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="F18" s="196">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="10" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="D18" s="197">
-        <v>0</v>
-      </c>
-      <c r="E18" s="197">
-        <v>0</v>
-      </c>
-      <c r="F18" s="197">
-        <v>0</v>
-      </c>
-      <c r="G18" s="198" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="199" t="s">
+      <c r="D19" s="197">
+        <v>0</v>
+      </c>
+      <c r="E19" s="197">
+        <v>0</v>
+      </c>
+      <c r="F19" s="197">
+        <v>0</v>
+      </c>
+      <c r="G19" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="199" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -35929,1629 +35935,1629 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="145" t="s">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="145" t="s">
         <v>817</v>
       </c>
-      <c r="C22" s="145"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="147" t="s">
+      <c r="C23" s="145"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="146"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="147" t="s">
         <v>804</v>
       </c>
-      <c r="D23" s="147" t="s">
+      <c r="D24" s="147" t="s">
         <v>818</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>819</v>
-      </c>
-      <c r="D24">
-        <v>0.90846119467638486</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D25">
-        <v>0.27162518208416181</v>
+        <v>0.90846119467638486</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D26">
-        <v>0.81726866046735724</v>
+        <v>0.27162518208416181</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D27">
-        <v>0.34079587723544508</v>
+        <v>0.81726866046735724</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D28">
-        <v>0.98824799370521366</v>
+        <v>0.34079587723544508</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D29">
-        <v>0.32106107116202942</v>
+        <v>0.98824799370521366</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>829</v>
+      </c>
+      <c r="D30">
+        <v>0.32106107116202942</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>831</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>0.93371384168102334</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
         <v>832</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C31" s="200" t="s">
-        <v>810</v>
-      </c>
-      <c r="D31">
-        <v>0.30414650929322951</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>833</v>
-      </c>
-      <c r="J31" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="200" t="s">
-        <v>835</v>
+        <v>810</v>
       </c>
       <c r="D32">
-        <v>0.3005775852039263</v>
+        <v>0.30414650929322951</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>836</v>
+        <v>833</v>
+      </c>
+      <c r="J32" t="s">
+        <v>834</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="200" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D33">
-        <v>0.76894809380036488</v>
+        <v>0.3005775852039263</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="200" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="D34">
-        <v>0.68887316941081111</v>
+        <v>0.76894809380036488</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="200" t="s">
+        <v>839</v>
+      </c>
+      <c r="D35">
+        <v>0.68887316941081111</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="200" t="s">
         <v>841</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>0.98074985450505592</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E36" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>843</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>0.86639443520588644</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
         <v>844</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="200" t="s">
-        <v>845</v>
-      </c>
-      <c r="D37">
-        <v>1.0571694859545731</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="200" t="s">
+        <v>845</v>
+      </c>
+      <c r="D38">
+        <v>1.0571694859545731</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="200" t="s">
         <v>847</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>0.80855622883571299</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
         <v>848</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>849</v>
-      </c>
-      <c r="D39">
-        <v>-2.469106618633899E-2</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F39" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D40">
-        <v>-2.3922206141805489E-2</v>
+        <v>-2.469106618633899E-2</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D41">
-        <v>0.94032795019740478</v>
+        <v>-2.3922206141805489E-2</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
+        <v>853</v>
+      </c>
+      <c r="D42">
+        <v>0.94032795019740478</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>855</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <v>0.94756863284113146</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="E43" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
         <v>856</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="200" t="s">
-        <v>857</v>
-      </c>
-      <c r="D43">
-        <v>1.11618130449523</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F43" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" s="200" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D44">
-        <v>0.29986416997635029</v>
+        <v>1.11618130449523</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" s="200" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D45">
-        <v>0.85762458634688188</v>
+        <v>0.29986416997635029</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" s="200" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D46">
-        <v>0.68887316941081111</v>
+        <v>0.85762458634688188</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" s="200" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D47">
-        <v>0.28381060228036231</v>
+        <v>0.68887316941081111</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" s="200" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D48">
-        <v>0.74393305058591253</v>
+        <v>0.28381060228036231</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="200" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D49">
-        <v>0.73855658713477379</v>
+        <v>0.74393305058591253</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="200" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D50">
-        <v>0.2281407609574547</v>
+        <v>0.73855658713477379</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C51" s="200" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D51">
-        <v>1.080763025022462</v>
+        <v>0.2281407609574547</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C52" s="200" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D52">
-        <v>0.32472440996417717</v>
+        <v>1.080763025022462</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C53" s="200" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="D53">
-        <v>1.1530177947591029</v>
+        <v>0.32472440996417717</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C54" s="200" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D54">
-        <v>0.34272991132433078</v>
+        <v>1.1530177947591029</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C55" s="200" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D55">
-        <v>1.0752379822602769</v>
+        <v>0.34272991132433078</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C56" s="200" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="D56">
-        <v>1.401266388048874</v>
+        <v>1.0752379822602769</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C57" s="200" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="D57">
-        <v>1.118530070618293</v>
+        <v>1.401266388048874</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C58" s="200" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D58">
-        <v>1.303923986127882</v>
+        <v>1.118530070618293</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C59" s="200" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D59">
-        <v>1.0006442771948729</v>
+        <v>1.303923986127882</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C60" s="200" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D60">
-        <v>1.2462675482169561</v>
+        <v>1.0006442771948729</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C61" s="200" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D61">
-        <v>1.0897093138445459</v>
+        <v>1.2462675482169561</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C62" s="200" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D62">
-        <v>1.429753986527831</v>
+        <v>1.0897093138445459</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C63" s="200" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="D63">
-        <v>1.3967298880817409</v>
+        <v>1.429753986527831</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C64" s="200" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D64">
-        <v>0.71641761358088285</v>
+        <v>1.3967298880817409</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="200" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="D65">
-        <v>0.74430956181877117</v>
+        <v>0.71641761358088285</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" s="200" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D66">
-        <v>0.67565438955443047</v>
+        <v>0.74430956181877117</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C67" s="200" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D67">
-        <v>0.86489647235226175</v>
+        <v>0.67565438955443047</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" s="200" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D68">
-        <v>0.7729540444011983</v>
+        <v>0.86489647235226175</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="200" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D69">
-        <v>0.81828559334530027</v>
+        <v>0.7729540444011983</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" s="200" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D70">
-        <v>-1.6482338753426171E-2</v>
+        <v>0.81828559334530027</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" s="200" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D71">
-        <v>-1.968146566187369E-2</v>
+        <v>-1.6482338753426171E-2</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C72" s="200" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D72">
-        <v>0.7671440380844482</v>
+        <v>-1.968146566187369E-2</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" s="200" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D73">
-        <v>0.79045397637937675</v>
+        <v>0.7671440380844482</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" s="200" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D74">
-        <v>0.93891783182266686</v>
+        <v>0.79045397637937675</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" s="200" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D75">
-        <v>1.3109337385351909</v>
+        <v>0.93891783182266686</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" s="200" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D76">
-        <v>0.66990379130299005</v>
+        <v>1.3109337385351909</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C77" s="200" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D77">
-        <v>0.74430956181877117</v>
+        <v>0.66990379130299005</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C78" s="200" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D78">
-        <v>0.87081341575373017</v>
+        <v>0.74430956181877117</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C79" s="200" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D79">
-        <v>0.57743502945375991</v>
+        <v>0.87081341575373017</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C80" s="200" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D80">
-        <v>0.57264949774480878</v>
+        <v>0.57743502945375991</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C81" s="200" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D81">
-        <v>0.71767543689007995</v>
+        <v>0.57264949774480878</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C82" s="200" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D82">
-        <v>0.92771399647553088</v>
+        <v>0.71767543689007995</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C83" s="200" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D83">
-        <v>1.3156757578908409</v>
+        <v>0.92771399647553088</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C84" s="200" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D84">
-        <v>1.2248001480370521</v>
+        <v>1.3156757578908409</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="85" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C85" s="200" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D85">
-        <v>1.6940404456869</v>
+        <v>1.2248001480370521</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C86" s="200" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D86">
-        <v>0.85801788671874712</v>
+        <v>1.6940404456869</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C87" s="200" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D87">
-        <v>0.19850002546049789</v>
+        <v>0.85801788671874712</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C88" s="200" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D88">
-        <v>0.74299742298240889</v>
+        <v>0.19850002546049789</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C89" s="200" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D89">
-        <v>0.27311459465307331</v>
+        <v>0.74299742298240889</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C90" s="200" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D90">
-        <v>0.98773021550772733</v>
+        <v>0.27311459465307331</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C91" s="200" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="D91">
-        <v>0.27403377599467038</v>
+        <v>0.98773021550772733</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C92" s="200" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D92">
-        <v>0.8713962312611806</v>
+        <v>0.27403377599467038</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="93" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C93" s="200" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="D93">
-        <v>0.22230949363166741</v>
+        <v>0.8713962312611806</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="94" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C94" s="200" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="D94">
-        <v>0.22582707554538209</v>
+        <v>0.22230949363166741</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="95" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C95" s="200" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D95">
-        <v>1.086848840216583</v>
+        <v>0.22582707554538209</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="96" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C96" s="200" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="D96">
-        <v>0.9333688927833228</v>
+        <v>1.086848840216583</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F96" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C97" s="200" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="D97">
-        <v>1.5443360451135639</v>
+        <v>0.9333688927833228</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="98" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C98" s="200" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="D98">
-        <v>1.006708468361317</v>
+        <v>1.5443360451135639</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C99" s="200" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D99">
-        <v>1.3826420349069539</v>
+        <v>1.006708468361317</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C100" s="200" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D100">
-        <v>1.0000938464838769</v>
+        <v>1.3826420349069539</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C101" s="200" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D101">
-        <v>-6.1588783514397128E-3</v>
+        <v>1.0000938464838769</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F101" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C102" s="200" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="D102">
-        <v>-3.7821679032148882E-3</v>
+        <v>-6.1588783514397128E-3</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C103" s="200" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="D103">
-        <v>1.248236672715392</v>
+        <v>-3.7821679032148882E-3</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="104" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C104" s="200" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D104">
-        <v>1.2348673245452491</v>
+        <v>1.248236672715392</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="105" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C105" s="200" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D105">
-        <v>1.2091874208164499</v>
+        <v>1.2348673245452491</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="106" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C106" s="200" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D106">
-        <v>0.23496619163846211</v>
+        <v>1.2091874208164499</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C107" s="200" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D107">
-        <v>1.303852461747784</v>
+        <v>0.23496619163846211</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F107" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C108" s="200" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D108">
-        <v>0.9333688927833228</v>
+        <v>1.303852461747784</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F108" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C109" s="200" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D109">
-        <v>0.34034355194690169</v>
+        <v>0.9333688927833228</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F109" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C110" s="200" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="D110">
-        <v>1.3061356696865201</v>
+        <v>0.34034355194690169</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F110" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C111" s="200" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="D111">
-        <v>1.3015189636018949</v>
+        <v>1.3061356696865201</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F111" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C112" s="200" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D112">
-        <v>0.34203772537735622</v>
+        <v>1.3015189636018949</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F112" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="113" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C113" s="200" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D113">
-        <v>1.186723923110615</v>
+        <v>0.34203772537735622</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F113" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="114" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C114" s="200" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D114">
-        <v>0.25419250804359678</v>
+        <v>1.186723923110615</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F114" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="115" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C115" s="200" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D115">
-        <v>0.96521396065861842</v>
+        <v>0.25419250804359678</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="116" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C116" s="200" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D116">
-        <v>0.21208816877826209</v>
+        <v>0.96521396065861842</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F116" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="117" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C117" s="200" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D117">
+        <v>0.21208816877826209</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F117" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C118" s="200" t="s">
         <v>1005</v>
       </c>
-      <c r="D117">
+      <c r="D118">
         <v>-13.34228187919463</v>
       </c>
-      <c r="E117" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F117" t="s">
+      <c r="E118" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F118" t="s">
         <v>1005</v>
-      </c>
-    </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
-        <v>1006</v>
-      </c>
-      <c r="D118">
-        <v>0.93891215680503748</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F118" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="119" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D119">
-        <v>0.73036120430356599</v>
+        <v>0.93891215680503748</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F119" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="120" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D120">
-        <v>0.90235654510735674</v>
+        <v>0.73036120430356599</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F120" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="121" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D121">
-        <v>0.79830318769400144</v>
+        <v>0.90235654510735674</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F121" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="122" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D122">
-        <v>0.99954397516295967</v>
+        <v>0.79830318769400144</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F122" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="123" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D123">
-        <v>0.86597437882091677</v>
+        <v>0.99954397516295967</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F123" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="124" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D124">
+        <v>0.86597437882091677</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F124" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="125" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
         <v>1018</v>
       </c>
-      <c r="D124">
+      <c r="D125">
         <v>0.92762722617788618</v>
       </c>
-      <c r="E124" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F124" t="s">
+      <c r="E125" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F125" t="s">
         <v>1019</v>
-      </c>
-    </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C125" s="200" t="s">
-        <v>1020</v>
-      </c>
-      <c r="D125">
-        <v>0.73569948928852247</v>
-      </c>
-      <c r="E125" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F125" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="126" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C126" s="200" t="s">
-        <v>808</v>
+        <v>1020</v>
       </c>
       <c r="D126">
-        <v>0.74758867389374639</v>
+        <v>0.73569948928852247</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F126" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="127" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C127" s="200" t="s">
+        <v>808</v>
+      </c>
+      <c r="D127">
+        <v>0.74758867389374639</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F127" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C128" s="200" t="s">
         <v>1023</v>
       </c>
-      <c r="D127">
+      <c r="D128">
         <v>1.4080629521787209</v>
       </c>
-      <c r="E127" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F127" t="s">
+      <c r="E128" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F128" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
         <v>1025</v>
       </c>
-      <c r="D128">
+      <c r="D129">
         <v>1.3512187322610889</v>
       </c>
-      <c r="E128" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F128" t="s">
+      <c r="E129" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F129" t="s">
         <v>1026</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C129" s="200" t="s">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C130" s="200" t="s">
         <v>1027</v>
       </c>
-      <c r="D129">
+      <c r="D130">
         <v>1.560117588861349</v>
       </c>
-      <c r="E129" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F129" t="s">
+      <c r="E130" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F130" t="s">
         <v>1028</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C130" t="s">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
         <v>1029</v>
       </c>
-      <c r="D130">
+      <c r="D131">
         <v>1.1643911735223791</v>
       </c>
-      <c r="E130" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F130" t="s">
+      <c r="E131" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F131" t="s">
         <v>1030</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C131" s="200" t="s">
-        <v>1031</v>
-      </c>
-      <c r="D131">
-        <v>1.303662046752992</v>
-      </c>
-      <c r="E131" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F131" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C132" s="200" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D132">
+        <v>1.303662046752992</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F132" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C133" s="200" t="s">
         <v>1033</v>
       </c>
-      <c r="D132">
+      <c r="D133">
         <v>1.2526113987618199</v>
       </c>
-      <c r="E132" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F132" t="s">
+      <c r="E133" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F133" t="s">
         <v>1034</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C133" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D133">
-        <v>1.220045320542313E-2</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F133" t="s">
-        <v>1036</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C134" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D134">
-        <v>1.224590520189844E-2</v>
+        <v>1.220045320542313E-2</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F134" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="D135">
-        <v>1.326487160221423</v>
+        <v>1.224590520189844E-2</v>
       </c>
       <c r="E135" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F135" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D136">
+        <v>1.326487160221423</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F136" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
         <v>1041</v>
       </c>
-      <c r="D136">
+      <c r="D137">
         <v>1.3154980006997969</v>
       </c>
-      <c r="E136" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F136" t="s">
+      <c r="E137" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F137" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C137" s="10" t="s">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C138" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="D137" s="197">
-        <v>0</v>
-      </c>
-      <c r="E137" s="198" t="s">
-        <v>0</v>
-      </c>
-      <c r="F137" s="199" t="s">
+      <c r="D138" s="197">
+        <v>0</v>
+      </c>
+      <c r="E138" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="F138" s="199" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -37560,90 +37566,90 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B141" s="145" t="s">
+      <c r="A141" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="145" t="s">
         <v>1043</v>
       </c>
-      <c r="C141" s="145"/>
-      <c r="D141" s="146"/>
-      <c r="E141" s="146"/>
-      <c r="F141" s="146"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C142" s="147" t="s">
+      <c r="C142" s="145"/>
+      <c r="D142" s="146"/>
+      <c r="E142" s="146"/>
+      <c r="F142" s="146"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C143" s="147" t="s">
         <v>1044</v>
       </c>
-      <c r="D142" s="147" t="s">
+      <c r="D143" s="147" t="s">
         <v>1045</v>
       </c>
-      <c r="E142" s="147" t="s">
+      <c r="E143" s="147" t="s">
         <v>1046</v>
       </c>
-      <c r="F142" s="201" t="s">
+      <c r="F143" s="201" t="s">
         <v>1047</v>
       </c>
-      <c r="G142" s="201" t="s">
+      <c r="G143" s="201" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C143" s="1" t="s">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C144" s="1" t="s">
         <v>1049</v>
       </c>
-      <c r="D143" s="61">
+      <c r="D144" s="61">
         <v>-999</v>
       </c>
-      <c r="E143" s="61">
+      <c r="E144" s="61">
         <v>-999</v>
       </c>
-      <c r="F143" s="1">
+      <c r="F144" s="1">
         <v>6</v>
       </c>
-      <c r="G143" s="1">
+      <c r="G144" s="1">
         <v>22</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C144" s="202" t="s">
-        <v>1050</v>
-      </c>
-      <c r="D144" s="1">
-        <v>6</v>
-      </c>
-      <c r="E144" s="1">
-        <v>1</v>
-      </c>
-      <c r="F144" s="196">
-        <v>1.7772312730847999</v>
-      </c>
-      <c r="G144" s="196">
-        <v>6.5165146679776598</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C145" s="202" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D145" s="1">
+        <v>6</v>
+      </c>
+      <c r="E145" s="1">
+        <v>1</v>
+      </c>
+      <c r="F145" s="196">
+        <v>1.7772312730847999</v>
+      </c>
+      <c r="G145" s="196">
+        <v>6.5165146679776598</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C146" s="202" t="s">
         <v>1051</v>
       </c>
-      <c r="D145" s="1">
+      <c r="D146" s="1">
         <v>22</v>
       </c>
-      <c r="E145" s="1">
+      <c r="E146" s="1">
         <v>2.4</v>
       </c>
-      <c r="F145" s="196">
+      <c r="F146" s="196">
         <v>2.1046299727964199</v>
       </c>
-      <c r="G145" s="196">
+      <c r="G146" s="196">
         <v>7.7169765669202297</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
@@ -37655,42 +37661,20 @@
       <c r="A149" t="s">
         <v>0</v>
       </c>
-      <c r="F149" s="24" t="s">
-        <v>1052</v>
-      </c>
-      <c r="G149" s="24" t="s">
-        <v>1053</v>
-      </c>
-      <c r="H149" s="24" t="s">
-        <v>1054</v>
-      </c>
-      <c r="I149" s="24"/>
-      <c r="J149" s="24"/>
-      <c r="K149" s="24"/>
-      <c r="L149" s="24"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>0</v>
       </c>
-      <c r="C150" s="24" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D150" s="203" t="s">
-        <v>1056</v>
-      </c>
-      <c r="E150" s="6">
-        <v>19</v>
-      </c>
-      <c r="F150" s="24">
-        <f>(E150-F154)/(G154-F154)</f>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="G150" s="24">
-        <f>F155+(F150*(G155-F155))</f>
-        <v>5.4825862512771142</v>
-      </c>
-      <c r="H150" s="24"/>
+      <c r="F150" s="24" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G150" s="24" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H150" s="24" t="s">
+        <v>1054</v>
+      </c>
       <c r="I150" s="24"/>
       <c r="J150" s="24"/>
       <c r="K150" s="24"/>
@@ -37700,187 +37684,209 @@
       <c r="A151" t="s">
         <v>0</v>
       </c>
-      <c r="C151" s="24"/>
+      <c r="C151" s="24" t="s">
+        <v>1055</v>
+      </c>
       <c r="D151" s="203" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E151" s="6">
-        <v>1.4615400000000001</v>
+        <v>19</v>
       </c>
       <c r="F151" s="24">
-        <f>(E151-E155)/(E156-E155)</f>
-        <v>0.61785809906291833</v>
+        <f>(E151-F155)/(G155-F155)</f>
+        <v>0.47619047619047616</v>
       </c>
       <c r="G151" s="24">
-        <f>F156+(F150*(G156-F156))</f>
-        <v>8.1335991195659769</v>
-      </c>
-      <c r="H151" s="24">
-        <f>G150+(F151*(G151-G150))</f>
-        <v>7.1205360226694054</v>
-      </c>
+        <f>F156+(F151*(G156-F156))</f>
+        <v>5.4825862512771142</v>
+      </c>
+      <c r="H151" s="24"/>
       <c r="I151" s="24"/>
       <c r="J151" s="24"/>
       <c r="K151" s="24"/>
       <c r="L151" s="24"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B152" s="145" t="s">
+      <c r="A152" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" s="24"/>
+      <c r="D152" s="203" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E152" s="6">
+        <v>1.4615400000000001</v>
+      </c>
+      <c r="F152" s="24">
+        <f>(E152-E156)/(E157-E156)</f>
+        <v>0.61785809906291833</v>
+      </c>
+      <c r="G152" s="24">
+        <f>F157+(F151*(G157-F157))</f>
+        <v>8.1335991195659769</v>
+      </c>
+      <c r="H152" s="24">
+        <f>G151+(F152*(G152-G151))</f>
+        <v>7.1205360226694054</v>
+      </c>
+      <c r="I152" s="24"/>
+      <c r="J152" s="24"/>
+      <c r="K152" s="24"/>
+      <c r="L152" s="24"/>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B153" s="145" t="s">
         <v>1058</v>
       </c>
-      <c r="C152" s="145"/>
-      <c r="D152" s="146"/>
-      <c r="E152" s="146"/>
-      <c r="F152" s="146"/>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C153" s="147" t="s">
+      <c r="C153" s="145"/>
+      <c r="D153" s="146"/>
+      <c r="E153" s="146"/>
+      <c r="F153" s="146"/>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C154" s="147" t="s">
         <v>1044</v>
       </c>
-      <c r="D153" s="147" t="s">
+      <c r="D154" s="147" t="s">
         <v>1045</v>
       </c>
-      <c r="E153" s="147" t="s">
+      <c r="E154" s="147" t="s">
         <v>1046</v>
       </c>
-      <c r="F153" s="201" t="s">
+      <c r="F154" s="201" t="s">
         <v>1047</v>
       </c>
-      <c r="G153" s="201" t="s">
+      <c r="G154" s="201" t="s">
         <v>1048</v>
       </c>
-      <c r="H153" s="201" t="s">
+      <c r="H154" s="201" t="s">
         <v>1059</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C154" s="1" t="s">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C155" s="1" t="s">
         <v>1049</v>
       </c>
-      <c r="D154" s="61">
+      <c r="D155" s="61">
         <v>-999</v>
       </c>
-      <c r="E154" s="61">
+      <c r="E155" s="61">
         <v>-999</v>
       </c>
-      <c r="F154" s="1">
+      <c r="F155" s="1">
         <v>14</v>
       </c>
-      <c r="G154" s="1">
+      <c r="G155" s="1">
         <v>24.5</v>
       </c>
-      <c r="H154" s="1">
+      <c r="H155" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C155" s="202" t="s">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C156" s="202" t="s">
         <v>1050</v>
       </c>
-      <c r="D155" s="204">
+      <c r="D156" s="204">
         <v>14</v>
       </c>
-      <c r="E155" s="205">
-        <v>1</v>
-      </c>
-      <c r="F155" s="206">
+      <c r="E156" s="205">
+        <v>1</v>
+      </c>
+      <c r="F156" s="206">
         <v>4.0472407657688896</v>
       </c>
-      <c r="G155" s="206">
+      <c r="G156" s="206">
         <v>7.0614662853361603</v>
       </c>
-      <c r="H155" s="206">
+      <c r="H156" s="206">
         <v>10.0579689809278</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C156" s="207" t="s">
-        <v>1048</v>
-      </c>
-      <c r="D156" s="61">
-        <v>-999</v>
-      </c>
-      <c r="E156" s="205">
-        <v>1.7470000000000001</v>
-      </c>
-      <c r="F156" s="206">
-        <v>6.1745806457053201</v>
-      </c>
-      <c r="G156" s="206">
-        <v>10.288519440812699</v>
-      </c>
-      <c r="H156" s="206">
-        <v>14.0528614685423</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C157" s="207" t="s">
-        <v>1059</v>
+        <v>1048</v>
       </c>
       <c r="D157" s="61">
         <v>-999</v>
       </c>
       <c r="E157" s="205">
-        <v>2.12</v>
+        <v>1.7470000000000001</v>
       </c>
       <c r="F157" s="206">
-        <v>14.2402417304402</v>
+        <v>6.1745806457053201</v>
       </c>
       <c r="G157" s="206">
-        <v>23.261833752330102</v>
+        <v>10.288519440812699</v>
       </c>
       <c r="H157" s="206">
-        <v>30.962188370029502</v>
+        <v>14.0528614685423</v>
       </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C158" s="207" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D158" s="61">
         <v>-999</v>
       </c>
       <c r="E158" s="205">
+        <v>2.12</v>
+      </c>
+      <c r="F158" s="206">
+        <v>14.2402417304402</v>
+      </c>
+      <c r="G158" s="206">
+        <v>23.261833752330102</v>
+      </c>
+      <c r="H158" s="206">
+        <v>30.962188370029502</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C159" s="207" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D159" s="61">
+        <v>-999</v>
+      </c>
+      <c r="E159" s="205">
         <v>2.3069999999999999</v>
       </c>
-      <c r="F158" s="206">
+      <c r="F159" s="206">
         <v>19.5080882760811</v>
       </c>
-      <c r="G158" s="206">
+      <c r="G159" s="206">
         <v>31.842461807964899</v>
       </c>
-      <c r="H158" s="206">
+      <c r="H159" s="206">
         <v>42.388314683006897</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C159" s="202" t="s">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C160" s="202" t="s">
         <v>1051</v>
       </c>
-      <c r="D159" s="204">
+      <c r="D160" s="204">
         <v>35</v>
       </c>
-      <c r="E159" s="205">
+      <c r="E160" s="205">
         <v>2.4</v>
       </c>
-      <c r="F159" s="206">
+      <c r="F160" s="206">
         <v>23.0287784144776</v>
       </c>
-      <c r="G159" s="206">
+      <c r="G160" s="206">
         <v>37.512878873992399</v>
       </c>
-      <c r="H159" s="206">
+      <c r="H160" s="206">
         <v>49.8631679938944</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
@@ -37889,204 +37895,204 @@
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B163" s="145" t="s">
+      <c r="A163" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B164" s="145" t="s">
         <v>1061</v>
       </c>
-      <c r="C163" s="145"/>
-      <c r="D163" s="146"/>
-      <c r="E163" s="146"/>
-      <c r="F163" s="146"/>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C164" s="147" t="s">
+      <c r="C164" s="145"/>
+      <c r="D164" s="146"/>
+      <c r="E164" s="146"/>
+      <c r="F164" s="146"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C165" s="147" t="s">
         <v>1044</v>
       </c>
-      <c r="D164" s="147" t="s">
+      <c r="D165" s="147" t="s">
         <v>1062</v>
       </c>
-      <c r="E164" s="147" t="s">
+      <c r="E165" s="147" t="s">
         <v>1063</v>
       </c>
-      <c r="F164" s="201" t="s">
+      <c r="F165" s="201" t="s">
         <v>1047</v>
       </c>
-      <c r="G164" s="201" t="s">
+      <c r="G165" s="201" t="s">
         <v>1048</v>
       </c>
-      <c r="H164" s="201" t="s">
+      <c r="H165" s="201" t="s">
         <v>1059</v>
       </c>
-      <c r="I164" s="201" t="s">
+      <c r="I165" s="201" t="s">
         <v>1060</v>
       </c>
-      <c r="J164" s="201" t="s">
+      <c r="J165" s="201" t="s">
         <v>1064</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C165" s="1" t="s">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C166" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="D165" s="61">
+      <c r="D166" s="61">
         <v>-999</v>
       </c>
-      <c r="E165" s="61">
+      <c r="E166" s="61">
         <v>-999</v>
       </c>
-      <c r="F165" s="1">
+      <c r="F166" s="1">
         <v>5</v>
       </c>
-      <c r="G165" s="1">
+      <c r="G166" s="1">
         <v>6.5</v>
       </c>
-      <c r="H165" s="1">
+      <c r="H166" s="1">
         <v>8</v>
       </c>
-      <c r="I165" s="1">
+      <c r="I166" s="1">
         <v>9.5</v>
       </c>
-      <c r="J165" s="1">
+      <c r="J166" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C166" s="202" t="s">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C167" s="202" t="s">
         <v>1050</v>
       </c>
-      <c r="D166" s="204">
+      <c r="D167" s="204">
         <v>5</v>
       </c>
-      <c r="E166" s="205">
+      <c r="E167" s="205">
         <v>0.5</v>
       </c>
-      <c r="F166" s="206">
+      <c r="F167" s="206">
         <v>1.97075256891674</v>
       </c>
-      <c r="G166" s="206">
+      <c r="G167" s="206">
         <v>2.8444383206836301</v>
       </c>
-      <c r="H166" s="206">
+      <c r="H167" s="206">
         <v>3.9326226591917002</v>
       </c>
-      <c r="I166" s="206">
+      <c r="I167" s="206">
         <v>5.3269916570599696</v>
       </c>
-      <c r="J166" s="206">
+      <c r="J167" s="206">
         <v>7.1779300540934097</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C167" s="207" t="s">
-        <v>1048</v>
-      </c>
-      <c r="D167" s="61">
-        <v>-999</v>
-      </c>
-      <c r="E167" s="205">
-        <v>0.53300000000000003</v>
-      </c>
-      <c r="F167" s="206">
-        <v>1.96284432544732</v>
-      </c>
-      <c r="G167" s="206">
-        <v>2.8005516945156299</v>
-      </c>
-      <c r="H167" s="206">
-        <v>3.8193107805482698</v>
-      </c>
-      <c r="I167" s="206">
-        <v>5.0849283328115904</v>
-      </c>
-      <c r="J167" s="206">
-        <v>6.6994992979074697</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C168" s="207" t="s">
-        <v>1059</v>
+        <v>1048</v>
       </c>
       <c r="D168" s="61">
         <v>-999</v>
       </c>
       <c r="E168" s="205">
-        <v>0.6</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="F168" s="206">
-        <v>1.9458491393528901</v>
+        <v>1.96284432544732</v>
       </c>
       <c r="G168" s="206">
-        <v>2.7204932493267502</v>
+        <v>2.8005516945156299</v>
       </c>
       <c r="H168" s="206">
-        <v>3.6215925755201099</v>
+        <v>3.8193107805482698</v>
       </c>
       <c r="I168" s="206">
-        <v>4.68286348872397</v>
+        <v>5.0849283328115904</v>
       </c>
       <c r="J168" s="206">
-        <v>5.9511778179594499</v>
+        <v>6.6994992979074697</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C169" s="207" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D169" s="61">
         <v>-999</v>
       </c>
       <c r="E169" s="205">
+        <v>0.6</v>
+      </c>
+      <c r="F169" s="206">
+        <v>1.9458491393528901</v>
+      </c>
+      <c r="G169" s="206">
+        <v>2.7204932493267502</v>
+      </c>
+      <c r="H169" s="206">
+        <v>3.6215925755201099</v>
+      </c>
+      <c r="I169" s="206">
+        <v>4.68286348872397</v>
+      </c>
+      <c r="J169" s="206">
+        <v>5.9511778179594499</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C170" s="207" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D170" s="61">
+        <v>-999</v>
+      </c>
+      <c r="E170" s="205">
         <v>0.73299999999999998</v>
       </c>
-      <c r="F169" s="206">
+      <c r="F170" s="206">
         <v>1.9150348596070901</v>
       </c>
-      <c r="G169" s="206">
+      <c r="G170" s="206">
         <v>2.5886355631293001</v>
       </c>
-      <c r="H169" s="206">
+      <c r="H170" s="206">
         <v>3.31808108043731</v>
       </c>
-      <c r="I169" s="206">
+      <c r="I170" s="206">
         <v>4.1106164511500101</v>
       </c>
-      <c r="J169" s="206">
+      <c r="J170" s="206">
         <v>4.9747966105752699</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C170" s="202" t="s">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C171" s="202" t="s">
         <v>1051</v>
       </c>
-      <c r="D170" s="204">
+      <c r="D171" s="204">
         <v>11</v>
       </c>
-      <c r="E170" s="205">
-        <v>1</v>
-      </c>
-      <c r="F170" s="206">
+      <c r="E171" s="205">
+        <v>1</v>
+      </c>
+      <c r="F171" s="206">
         <v>1.9042669937369301</v>
       </c>
-      <c r="G170" s="206">
+      <c r="G171" s="206">
         <v>2.49795552472336</v>
       </c>
-      <c r="H170" s="206">
+      <c r="H171" s="206">
         <v>3.10249026657586</v>
       </c>
-      <c r="I170" s="206">
+      <c r="I171" s="206">
         <v>3.7181711866689202</v>
       </c>
-      <c r="J170" s="206">
+      <c r="J171" s="206">
         <v>4.3453094166638202</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
@@ -38095,204 +38101,204 @@
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B174" s="145" t="s">
+      <c r="A174" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B175" s="145" t="s">
         <v>1066</v>
       </c>
-      <c r="C174" s="145"/>
-      <c r="D174" s="146"/>
-      <c r="E174" s="146"/>
-      <c r="F174" s="146"/>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C175" s="147" t="s">
+      <c r="C175" s="145"/>
+      <c r="D175" s="146"/>
+      <c r="E175" s="146"/>
+      <c r="F175" s="146"/>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C176" s="147" t="s">
         <v>1044</v>
       </c>
-      <c r="D175" s="147" t="s">
+      <c r="D176" s="147" t="s">
         <v>1062</v>
       </c>
-      <c r="E175" s="147" t="s">
+      <c r="E176" s="147" t="s">
         <v>1063</v>
       </c>
-      <c r="F175" s="201" t="s">
+      <c r="F176" s="201" t="s">
         <v>1047</v>
       </c>
-      <c r="G175" s="201" t="s">
+      <c r="G176" s="201" t="s">
         <v>1048</v>
       </c>
-      <c r="H175" s="201" t="s">
+      <c r="H176" s="201" t="s">
         <v>1059</v>
       </c>
-      <c r="I175" s="201" t="s">
+      <c r="I176" s="201" t="s">
         <v>1060</v>
       </c>
-      <c r="J175" s="201" t="s">
+      <c r="J176" s="201" t="s">
         <v>1064</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C176" s="1" t="s">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C177" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="D176" s="61">
+      <c r="D177" s="61">
         <v>-999</v>
       </c>
-      <c r="E176" s="61">
+      <c r="E177" s="61">
         <v>-999</v>
       </c>
-      <c r="F176" s="1">
+      <c r="F177" s="1">
         <v>5</v>
       </c>
-      <c r="G176" s="1">
+      <c r="G177" s="1">
         <v>6.5</v>
       </c>
-      <c r="H176" s="1">
+      <c r="H177" s="1">
         <v>8</v>
       </c>
-      <c r="I176" s="1">
+      <c r="I177" s="1">
         <v>9.5</v>
       </c>
-      <c r="J176" s="1">
+      <c r="J177" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C177" s="202" t="s">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C178" s="202" t="s">
         <v>1050</v>
       </c>
-      <c r="D177" s="204">
+      <c r="D178" s="204">
         <v>5</v>
       </c>
-      <c r="E177" s="205">
+      <c r="E178" s="205">
         <v>0.5</v>
       </c>
-      <c r="F177" s="206">
-        <v>1.79088568325965</v>
-      </c>
-      <c r="G177" s="206">
-        <v>2.5867817149954102</v>
-      </c>
-      <c r="H177" s="206">
-        <v>3.5758024515454498</v>
-      </c>
-      <c r="I177" s="206">
-        <v>4.8426266640532498</v>
-      </c>
-      <c r="J177" s="206">
-        <v>6.5234260615100101</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C178" s="207" t="s">
-        <v>1048</v>
-      </c>
-      <c r="D178" s="61">
-        <v>-999</v>
-      </c>
-      <c r="E178" s="205">
-        <v>0.53300000000000003</v>
-      </c>
       <c r="F178" s="206">
-        <v>1.7754184510431199</v>
+        <v>1.7942855944084</v>
       </c>
       <c r="G178" s="206">
-        <v>2.5352521639685199</v>
+        <v>2.5916448771333802</v>
       </c>
       <c r="H178" s="206">
-        <v>3.4569741750052798</v>
+        <v>3.5825249774526</v>
       </c>
       <c r="I178" s="206">
-        <v>4.60164866838445</v>
+        <v>4.8517308256082803</v>
       </c>
       <c r="J178" s="206">
-        <v>6.0612992212070598</v>
+        <v>6.5356901340632803</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C179" s="207" t="s">
-        <v>1059</v>
+        <v>1048</v>
       </c>
       <c r="D179" s="61">
         <v>-999</v>
       </c>
       <c r="E179" s="205">
-        <v>0.6</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="F179" s="206">
-        <v>1.75272498581222</v>
+        <v>1.77898616093772</v>
       </c>
       <c r="G179" s="206">
-        <v>2.4510469309789502</v>
+        <v>2.5402916834371498</v>
       </c>
       <c r="H179" s="206">
-        <v>3.2624773122950899</v>
+        <v>3.4638458735704498</v>
       </c>
       <c r="I179" s="206">
-        <v>4.2178718940252597</v>
+        <v>4.6107957261729098</v>
       </c>
       <c r="J179" s="206">
-        <v>5.3592735577279402</v>
+        <v>6.0733477408235998</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C180" s="207" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D180" s="61">
         <v>-999</v>
       </c>
       <c r="E180" s="205">
+        <v>0.6</v>
+      </c>
+      <c r="F180" s="206">
+        <v>1.75659272239308</v>
+      </c>
+      <c r="G180" s="206">
+        <v>2.4563861478715201</v>
+      </c>
+      <c r="H180" s="206">
+        <v>3.2695841015439102</v>
+      </c>
+      <c r="I180" s="206">
+        <v>4.2270598588017201</v>
+      </c>
+      <c r="J180" s="206">
+        <v>5.3709478849509997</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C181" s="207" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D181" s="61">
+        <v>-999</v>
+      </c>
+      <c r="E181" s="205">
         <v>0.73299999999999998</v>
       </c>
-      <c r="F180" s="206">
-        <v>1.7160437881453801</v>
-      </c>
-      <c r="G180" s="206">
-        <v>2.3194022408452999</v>
-      </c>
-      <c r="H180" s="206">
-        <v>2.9726363183632198</v>
-      </c>
-      <c r="I180" s="206">
-        <v>3.6821969781279802</v>
-      </c>
-      <c r="J180" s="206">
-        <v>4.4556977991213698</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C181" s="202" t="s">
+      <c r="F181" s="206">
+        <v>1.72032382138787</v>
+      </c>
+      <c r="G181" s="206">
+        <v>2.32518712743276</v>
+      </c>
+      <c r="H181" s="206">
+        <v>2.9800504544991</v>
+      </c>
+      <c r="I181" s="206">
+        <v>3.6913808495307201</v>
+      </c>
+      <c r="J181" s="206">
+        <v>4.46681088075161</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C182" s="202" t="s">
         <v>1051</v>
       </c>
-      <c r="D181" s="204">
+      <c r="D182" s="204">
         <v>11</v>
       </c>
-      <c r="E181" s="205">
-        <v>1</v>
-      </c>
-      <c r="F181" s="206">
-        <v>1.6539168354304801</v>
-      </c>
-      <c r="G181" s="206">
-        <v>2.1693762782338699</v>
-      </c>
-      <c r="H181" s="206">
-        <v>2.6941658196721301</v>
-      </c>
-      <c r="I181" s="206">
-        <v>3.2285410931517098</v>
-      </c>
-      <c r="J181" s="206">
-        <v>3.77276715688292</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
+      <c r="E182" s="205">
+        <v>1</v>
+      </c>
+      <c r="F182" s="206">
+        <v>1.65911382447797</v>
+      </c>
+      <c r="G182" s="206">
+        <v>2.1761929600139598</v>
+      </c>
+      <c r="H182" s="206">
+        <v>2.7026315115116599</v>
+      </c>
+      <c r="I182" s="206">
+        <v>3.2386859156367702</v>
+      </c>
+      <c r="J182" s="206">
+        <v>3.7846220634737802</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
@@ -38301,208 +38307,213 @@
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B185" s="145" t="s">
+      <c r="A185" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B186" s="145" t="s">
         <v>1067</v>
       </c>
-      <c r="C185" s="145"/>
-      <c r="D185" s="146"/>
-      <c r="E185" s="146"/>
-      <c r="F185" s="146"/>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C186" s="147" t="s">
+      <c r="C186" s="145"/>
+      <c r="D186" s="146"/>
+      <c r="E186" s="146"/>
+      <c r="F186" s="146"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C187" s="147" t="s">
         <v>1044</v>
       </c>
-      <c r="D186" s="147" t="s">
+      <c r="D187" s="147" t="s">
         <v>1062</v>
       </c>
-      <c r="E186" s="147" t="s">
+      <c r="E187" s="147" t="s">
         <v>1063</v>
       </c>
-      <c r="F186" s="201" t="s">
+      <c r="F187" s="201" t="s">
         <v>1047</v>
       </c>
-      <c r="G186" s="201" t="s">
+      <c r="G187" s="201" t="s">
         <v>1048</v>
       </c>
-      <c r="H186" s="201" t="s">
+      <c r="H187" s="201" t="s">
         <v>1059</v>
       </c>
-      <c r="I186" s="201" t="s">
+      <c r="I187" s="201" t="s">
         <v>1060</v>
       </c>
-      <c r="J186" s="201" t="s">
+      <c r="J187" s="201" t="s">
         <v>1064</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C187" s="1" t="s">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C188" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="D187" s="61">
+      <c r="D188" s="61">
         <v>-999</v>
       </c>
-      <c r="E187" s="61">
+      <c r="E188" s="61">
         <v>-999</v>
       </c>
-      <c r="F187" s="1">
+      <c r="F188" s="1">
         <v>7</v>
       </c>
-      <c r="G187" s="1">
+      <c r="G188" s="1">
         <v>9.25</v>
       </c>
-      <c r="H187" s="1">
+      <c r="H188" s="1">
         <v>11.5</v>
       </c>
-      <c r="I187" s="1">
+      <c r="I188" s="1">
         <v>13.75</v>
       </c>
-      <c r="J187" s="1">
+      <c r="J188" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C188" s="202" t="s">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C189" s="202" t="s">
         <v>1050</v>
       </c>
-      <c r="D188" s="204">
+      <c r="D189" s="204">
         <v>7</v>
       </c>
-      <c r="E188" s="205">
+      <c r="E189" s="205">
         <v>0.5</v>
       </c>
-      <c r="F188" s="206">
-        <v>2.7016273330016198</v>
-      </c>
-      <c r="G188" s="206">
-        <v>4.0495852173573104</v>
-      </c>
-      <c r="H188" s="206">
-        <v>5.7957973330219099</v>
-      </c>
-      <c r="I188" s="206">
-        <v>8.2024235372696896</v>
-      </c>
-      <c r="J188" s="206">
-        <v>11.6886196227955</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C189" s="207" t="s">
-        <v>1048</v>
-      </c>
-      <c r="D189" s="61">
-        <v>-999</v>
-      </c>
-      <c r="E189" s="205">
-        <v>0.54</v>
-      </c>
       <c r="F189" s="206">
-        <v>2.6198635152546301</v>
+        <v>2.7615174522980399</v>
       </c>
       <c r="G189" s="206">
-        <v>3.8322414514425098</v>
+        <v>4.1485710088989096</v>
       </c>
       <c r="H189" s="206">
-        <v>5.3410425089460203</v>
+        <v>5.9340351273548704</v>
       </c>
       <c r="I189" s="206">
-        <v>7.2646659093057</v>
+        <v>8.3924622983812895</v>
       </c>
       <c r="J189" s="206">
-        <v>9.8004285599386698</v>
+        <v>11.947880320460801</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C190" s="207" t="s">
-        <v>1059</v>
+        <v>1048</v>
       </c>
       <c r="D190" s="61">
         <v>-999</v>
       </c>
       <c r="E190" s="205">
-        <v>0.62</v>
+        <v>0.54</v>
       </c>
       <c r="F190" s="206">
-        <v>2.49270666820766</v>
+        <v>2.6956190656579899</v>
       </c>
       <c r="G190" s="206">
-        <v>3.50745123673298</v>
+        <v>3.9411009592583599</v>
       </c>
       <c r="H190" s="206">
-        <v>4.6627116304482996</v>
+        <v>5.4901821757658498</v>
       </c>
       <c r="I190" s="206">
-        <v>5.9896865405500597</v>
+        <v>7.4630673018686604</v>
       </c>
       <c r="J190" s="206">
-        <v>7.5294833005236503</v>
+        <v>10.060210076720599</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C191" s="207" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D191" s="61">
         <v>-999</v>
       </c>
       <c r="E191" s="205">
+        <v>0.62</v>
+      </c>
+      <c r="F191" s="206">
+        <v>2.57861527254442</v>
+      </c>
+      <c r="G191" s="206">
+        <v>3.6273512314369798</v>
+      </c>
+      <c r="H191" s="206">
+        <v>4.8206175932191604</v>
+      </c>
+      <c r="I191" s="206">
+        <v>6.1903363384175796</v>
+      </c>
+      <c r="J191" s="206">
+        <v>7.7785086506320402</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C192" s="207" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D192" s="61">
+        <v>-999</v>
+      </c>
+      <c r="E192" s="205">
         <v>0.78</v>
       </c>
-      <c r="F191" s="206">
-        <v>2.3643583391073602</v>
-      </c>
-      <c r="G191" s="206">
-        <v>3.1680836578940701</v>
-      </c>
-      <c r="H191" s="206">
-        <v>3.99457534438727</v>
-      </c>
-      <c r="I191" s="206">
-        <v>4.8447715247557497</v>
-      </c>
-      <c r="J191" s="206">
-        <v>5.7196590948597601</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C192" s="202" t="s">
+      <c r="F192" s="206">
+        <v>2.4666459333349202</v>
+      </c>
+      <c r="G192" s="206">
+        <v>3.3051087647532902</v>
+      </c>
+      <c r="H192" s="206">
+        <v>4.1673064794133801</v>
+      </c>
+      <c r="I192" s="206">
+        <v>5.0542179253575998</v>
+      </c>
+      <c r="J192" s="206">
+        <v>5.9668730023326901</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C193" s="202" t="s">
         <v>1051</v>
       </c>
-      <c r="D192" s="204">
+      <c r="D193" s="204">
         <v>16</v>
       </c>
-      <c r="E192" s="205">
+      <c r="E193" s="205">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F192" s="206">
-        <v>2.18223818437205</v>
-      </c>
-      <c r="G192" s="206">
-        <v>2.8749906050941898</v>
-      </c>
-      <c r="H192" s="206">
-        <v>3.56353949414199</v>
-      </c>
-      <c r="I192" s="206">
-        <v>4.2478967483252603</v>
-      </c>
-      <c r="J192" s="206">
-        <v>4.9280744439389403</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
+      <c r="F193" s="206">
+        <v>2.3452972083399901</v>
+      </c>
+      <c r="G193" s="206">
+        <v>3.0914418940374002</v>
+      </c>
+      <c r="H193" s="206">
+        <v>3.83384931080638</v>
+      </c>
+      <c r="I193" s="206">
+        <v>4.5725249664643197</v>
+      </c>
+      <c r="J193" s="206">
+        <v>5.3074744820016102</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>